<commit_message>
Added my story cards
</commit_message>
<xml_diff>
--- a/Release, Sprint and Story Cards/Task Assignment Table - Sprint 2.xlsx
+++ b/Release, Sprint and Story Cards/Task Assignment Table - Sprint 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoon\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xero\IFB299\Release, Sprint and Story Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>Task Assignment - Sprint 2</t>
   </si>
@@ -110,17 +110,23 @@
   <si>
     <t>Not Complete</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Braydon</t>
+  </si>
+  <si>
+    <t>Not Complete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -128,13 +134,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -487,24 +493,24 @@
   <dimension ref="B2:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -521,7 +527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6">
       <c r="B4" s="2">
         <v>8</v>
       </c>
@@ -538,7 +544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -555,7 +561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6">
       <c r="B6" s="2">
         <v>9</v>
       </c>
@@ -572,7 +578,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6">
       <c r="B7" s="2">
         <v>10</v>
       </c>
@@ -589,7 +595,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -600,7 +606,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6">
       <c r="B9" s="3">
         <v>14</v>
       </c>
@@ -617,18 +623,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6">
       <c r="B10" s="3">
         <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
       <c r="F10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6">
       <c r="B11" s="3">
         <v>16</v>
       </c>
@@ -639,7 +651,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6">
       <c r="B12" s="3">
         <v>13</v>
       </c>
@@ -656,7 +668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6">
       <c r="B13" s="3">
         <v>17</v>
       </c>
@@ -667,23 +679,35 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6">
       <c r="B14" t="s">
         <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
       <c r="F14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6">
       <c r="B15" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
       </c>
       <c r="F15" t="s">
         <v>25</v>

</xml_diff>